<commit_message>
Respuestas finales planteadas (creación pdf)
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p4/P4_UO277876.xlsx
+++ b/src/main/java/algestudiante/p4/P4_UO277876.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F0AF02-299F-4B74-8B1F-DCDE30CE4511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFBCEC5-7F37-4FC5-BD20-A9A890531239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Devoradores" sheetId="5" r:id="rId1"/>
+    <sheet name="Devoradores (2)" sheetId="7" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>nVeces</t>
   </si>
@@ -85,6 +87,18 @@
   </si>
   <si>
     <t>nVeces = 10</t>
+  </si>
+  <si>
+    <t>Complejidad:</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>O(nlogn)</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -291,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -337,6 +351,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,64 +981,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.4E-3</c:v>
+                  <c:v>2.1700000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.97E-3</c:v>
+                  <c:v>3.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2500000000000003E-3</c:v>
+                  <c:v>7.9500000000000005E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2279999999999999E-2</c:v>
+                  <c:v>1.7430000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.681E-2</c:v>
+                  <c:v>3.7310000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6660000000000002E-2</c:v>
+                  <c:v>7.424E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12639</c:v>
+                  <c:v>0.17363000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24589</c:v>
+                  <c:v>0.35206999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53864000000000001</c:v>
+                  <c:v>0.82206000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.09412</c:v>
+                  <c:v>1.6734800000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3229000000000002</c:v>
+                  <c:v>3.0482999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7878999999999996</c:v>
+                  <c:v>7.5076000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.2875</c:v>
+                  <c:v>16.625599999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.116</c:v>
+                  <c:v>23.931000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46.942</c:v>
+                  <c:v>46.341999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>94.695999999999998</c:v>
+                  <c:v>83.436000000000007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>211.67</c:v>
+                  <c:v>150.39400000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>450.98</c:v>
+                  <c:v>259.54000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>910.41</c:v>
+                  <c:v>530.09</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1842.71</c:v>
+                  <c:v>1535.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1396,64 +1411,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.57E-3</c:v>
+                  <c:v>1.3500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2100000000000002E-3</c:v>
+                  <c:v>2.5500000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6600000000000001E-3</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4970000000000001E-2</c:v>
+                  <c:v>1.124E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1060000000000001E-2</c:v>
+                  <c:v>2.8080000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9630000000000006E-2</c:v>
+                  <c:v>5.491E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14329</c:v>
+                  <c:v>0.12195</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.28833999999999999</c:v>
+                  <c:v>0.24113999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63583000000000001</c:v>
+                  <c:v>0.51256999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.29514</c:v>
+                  <c:v>1.07199</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8111000000000002</c:v>
+                  <c:v>2.0118999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.6220999999999997</c:v>
+                  <c:v>4.1510999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.364100000000001</c:v>
+                  <c:v>10.758599999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.555</c:v>
+                  <c:v>27.904</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>56.088999999999999</c:v>
+                  <c:v>63.445</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>112.74</c:v>
+                  <c:v>110.086</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>250.26</c:v>
+                  <c:v>252.44</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>507.54</c:v>
+                  <c:v>508.56</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1068.18</c:v>
+                  <c:v>1112.03</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2394.6999999999998</c:v>
+                  <c:v>2741</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,6 +1477,1304 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-85F3-4233-93A6-4A4F49BA3469}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1821346863"/>
+        <c:axId val="1821344367"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1821346863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821344367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1821344367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821346863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40614749745877143"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1377865846239424E-2"/>
+          <c:y val="0.16245370370370371"/>
+          <c:w val="0.86248526881159726"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Devoradores (2)'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t(DEV1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Devoradores (2)'!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>819200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1638400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3276800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6553600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13107200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26214400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52428800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Devoradores (2)'!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.7100000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0800000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1640000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4229999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8630000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5499999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9602999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8151999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6614000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15032899999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.29681000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.60407</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.27176</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6665000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.3940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.739599999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.338999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44.255000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.495000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8189-4B79-B4DF-5BA07A293714}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1821346863"/>
+        <c:axId val="1821344367"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1821346863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821344367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1821344367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821346863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7041166557477007E-2"/>
+          <c:y val="0.15319444444444447"/>
+          <c:w val="0.84288557336926295"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Devoradores (2)'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t(DEV2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FFC000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Devoradores (2)'!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>819200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1638400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3276800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6553600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13107200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26214400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52428800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Devoradores (2)'!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.4E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.97E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2500000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2279999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.681E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6660000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12639</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24589</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53864000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.09412</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3229000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7878999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.2875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.116</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.942</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>94.695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>211.67</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>450.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>910.41</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1842.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C362-470C-B89B-CD0F2281226F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1821346863"/>
+        <c:axId val="1821344367"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1821346863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821344367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1821344367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821346863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7469816272965873E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.82686351706036743"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Devoradores (2)'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t(DEV3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Devoradores (2)'!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>819200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1638400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3276800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6553600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13107200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26214400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52428800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Devoradores (2)'!$E$3:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.57E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2100000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6600000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4970000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1060000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9630000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14329</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28833999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63583000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.29514</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8111000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.6220999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.364100000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56.088999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112.74</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250.26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>507.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1068.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2394.6999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6326-43F8-975D-81AE4EC14259}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1772,6 +3085,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2805,6 +4238,1554 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3417,6 +6398,125 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290CDC86-0C7C-4E79-AAD8-D754C49E99AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>937260</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73274002-F56D-4415-9F4A-F216545E5858}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1226820</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F88E80-7010-412F-AA89-22DE99518B95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DF756D-3203-4DE0-91F3-B0A6701DFFCB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3736,10 +6836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50AC779-C55D-4822-8A6D-58AA05F2A758}">
-  <dimension ref="A2:N22"/>
+  <dimension ref="A2:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3795,12 +6895,12 @@
         <v>1.7100000000000001E-4</v>
       </c>
       <c r="D3" s="20">
-        <f>140/N7</f>
-        <v>1.4E-3</v>
+        <f>217/N7</f>
+        <v>2.1700000000000001E-3</v>
       </c>
       <c r="E3" s="20">
-        <f>157/N7</f>
-        <v>1.57E-3</v>
+        <f>135/N7</f>
+        <v>1.3500000000000001E-3</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>12</v>
@@ -3826,12 +6926,12 @@
         <v>3.6000000000000002E-4</v>
       </c>
       <c r="D4" s="20">
-        <f>297/N7</f>
-        <v>2.97E-3</v>
+        <f>360/N7</f>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E4" s="20">
-        <f>421/N7</f>
-        <v>4.2100000000000002E-3</v>
+        <f>255/N7</f>
+        <v>2.5500000000000002E-3</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="24"/>
@@ -3853,12 +6953,12 @@
         <v>6.0800000000000003E-4</v>
       </c>
       <c r="D5" s="20">
-        <f>625/N7</f>
-        <v>6.2500000000000003E-3</v>
+        <f>795/N7</f>
+        <v>7.9500000000000005E-3</v>
       </c>
       <c r="E5" s="20">
-        <f>766/N7</f>
-        <v>7.6600000000000001E-3</v>
+        <f>540/N7</f>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="24"/>
@@ -3876,12 +6976,12 @@
         <v>1.1640000000000001E-3</v>
       </c>
       <c r="D6" s="20">
-        <f>1228/N7</f>
-        <v>1.2279999999999999E-2</v>
+        <f>1743/N7</f>
+        <v>1.7430000000000001E-2</v>
       </c>
       <c r="E6" s="20">
-        <f>1497/N7</f>
-        <v>1.4970000000000001E-2</v>
+        <f>1124/N7</f>
+        <v>1.124E-2</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="24"/>
@@ -3899,12 +6999,12 @@
         <v>2.4229999999999998E-3</v>
       </c>
       <c r="D7" s="20">
-        <f>2681/N7</f>
-        <v>2.681E-2</v>
+        <f>3731/N7</f>
+        <v>3.7310000000000003E-2</v>
       </c>
       <c r="E7" s="20">
-        <f>3106/N7</f>
-        <v>3.1060000000000001E-2</v>
+        <f>2808/N7</f>
+        <v>2.8080000000000001E-2</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="24"/>
@@ -3922,12 +7022,12 @@
         <v>4.8630000000000001E-3</v>
       </c>
       <c r="D8" s="20">
-        <f>5666/N7</f>
-        <v>5.6660000000000002E-2</v>
+        <f>7424/N7</f>
+        <v>7.424E-2</v>
       </c>
       <c r="E8" s="20">
-        <f>7963/N7</f>
-        <v>7.9630000000000006E-2</v>
+        <f>5491/N7</f>
+        <v>5.491E-2</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="24"/>
@@ -3945,12 +7045,12 @@
         <v>9.5499999999999995E-3</v>
       </c>
       <c r="D9" s="20">
-        <f>12639/N7</f>
-        <v>0.12639</v>
+        <f>17363/N7</f>
+        <v>0.17363000000000001</v>
       </c>
       <c r="E9" s="20">
-        <f>14329/N7</f>
-        <v>0.14329</v>
+        <f>12195/N7</f>
+        <v>0.12195</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="24"/>
@@ -3968,12 +7068,12 @@
         <v>1.9602999999999999E-2</v>
       </c>
       <c r="D10" s="20">
-        <f>24589/N7</f>
-        <v>0.24589</v>
+        <f>35207/N7</f>
+        <v>0.35206999999999999</v>
       </c>
       <c r="E10" s="20">
-        <f>28834/N7</f>
-        <v>0.28833999999999999</v>
+        <f>24114/N7</f>
+        <v>0.24113999999999999</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="24"/>
@@ -3991,12 +7091,12 @@
         <v>3.8151999999999998E-2</v>
       </c>
       <c r="D11" s="20">
-        <f>53864/N7</f>
-        <v>0.53864000000000001</v>
+        <f>82206/N7</f>
+        <v>0.82206000000000001</v>
       </c>
       <c r="E11" s="20">
-        <f>63583/N7</f>
-        <v>0.63583000000000001</v>
+        <f>51257/N7</f>
+        <v>0.51256999999999997</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="24"/>
@@ -4014,12 +7114,12 @@
         <v>7.6614000000000002E-2</v>
       </c>
       <c r="D12" s="20">
-        <f>109412/N7</f>
-        <v>1.09412</v>
+        <f>167348/N7</f>
+        <v>1.6734800000000001</v>
       </c>
       <c r="E12" s="20">
-        <f>129514/N7</f>
-        <v>1.29514</v>
+        <f>107199/N7</f>
+        <v>1.07199</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="24"/>
@@ -4037,18 +7137,21 @@
         <v>0.15032899999999999</v>
       </c>
       <c r="D13" s="20">
-        <f>23229/N8</f>
-        <v>2.3229000000000002</v>
+        <f>30483/N8</f>
+        <v>3.0482999999999998</v>
       </c>
       <c r="E13" s="20">
-        <f>28111/N8</f>
-        <v>2.8111000000000002</v>
+        <f>20119/N8</f>
+        <v>2.0118999999999998</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -4063,12 +7166,12 @@
         <v>0.29681000000000002</v>
       </c>
       <c r="D14" s="20">
-        <f>47879/N8</f>
-        <v>4.7878999999999996</v>
+        <f>75076/N8</f>
+        <v>7.5076000000000001</v>
       </c>
       <c r="E14" s="20">
-        <f>56221/N8</f>
-        <v>5.6220999999999997</v>
+        <f>41511/N8</f>
+        <v>4.1510999999999996</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="24"/>
@@ -4083,12 +7186,12 @@
         <v>0.60407</v>
       </c>
       <c r="D15" s="20">
-        <f>102875/N8</f>
-        <v>10.2875</v>
+        <f>166256/N8</f>
+        <v>16.625599999999999</v>
       </c>
       <c r="E15" s="20">
-        <f>123641/N8</f>
-        <v>12.364100000000001</v>
+        <f>107586/N8</f>
+        <v>10.758599999999999</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="24"/>
@@ -4103,12 +7206,12 @@
         <v>1.27176</v>
       </c>
       <c r="D16" s="20">
-        <f>23116/N9</f>
-        <v>23.116</v>
+        <f>23931/N9</f>
+        <v>23.931000000000001</v>
       </c>
       <c r="E16" s="20">
-        <f>25555/N9</f>
-        <v>25.555</v>
+        <f>27904/N9</f>
+        <v>27.904</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>14</v>
@@ -4129,12 +7232,12 @@
         <v>2.6665000000000001</v>
       </c>
       <c r="D17" s="20">
-        <f>46942/N9</f>
-        <v>46.942</v>
+        <f>46342/N9</f>
+        <v>46.341999999999999</v>
       </c>
       <c r="E17" s="20">
-        <f>56089/N9</f>
-        <v>56.088999999999999</v>
+        <f>63445/N9</f>
+        <v>63.445</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="24"/>
@@ -4149,12 +7252,12 @@
         <v>5.3940999999999999</v>
       </c>
       <c r="D18" s="20">
-        <f>94696/N9</f>
-        <v>94.695999999999998</v>
+        <f>83436/N9</f>
+        <v>83.436000000000007</v>
       </c>
       <c r="E18" s="20">
-        <f>112740/N9</f>
-        <v>112.74</v>
+        <f>110086/N9</f>
+        <v>110.086</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="24"/>
@@ -4169,6 +7272,540 @@
         <v>10.739599999999999</v>
       </c>
       <c r="D19" s="20">
+        <f>150394/N9</f>
+        <v>150.39400000000001</v>
+      </c>
+      <c r="E19" s="20">
+        <f>25244/N10</f>
+        <v>252.44</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="19">
+        <v>13107200</v>
+      </c>
+      <c r="C20" s="20">
+        <f>22339/N9</f>
+        <v>22.338999999999999</v>
+      </c>
+      <c r="D20" s="20">
+        <f>25954/N10</f>
+        <v>259.54000000000002</v>
+      </c>
+      <c r="E20" s="20">
+        <f>50856/N10</f>
+        <v>508.56</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="19">
+        <v>26214400</v>
+      </c>
+      <c r="C21" s="20">
+        <f>44255/N9</f>
+        <v>44.255000000000003</v>
+      </c>
+      <c r="D21" s="20">
+        <f>53009/N10</f>
+        <v>530.09</v>
+      </c>
+      <c r="E21" s="20">
+        <f>111203/N10</f>
+        <v>1112.03</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="21">
+        <v>52428800</v>
+      </c>
+      <c r="C22" s="22">
+        <f>89495/N9</f>
+        <v>89.495000000000005</v>
+      </c>
+      <c r="D22" s="22">
+        <f>153535/N10</f>
+        <v>1535.35</v>
+      </c>
+      <c r="E22" s="22">
+        <f>27410/N11</f>
+        <v>2741</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B50BAE-647B-4B47-9D7F-56C45E2EDA0E}">
+  <dimension ref="A2:N23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="17">
+        <v>100</v>
+      </c>
+      <c r="C3" s="20">
+        <f>171/N6</f>
+        <v>1.7100000000000001E-4</v>
+      </c>
+      <c r="D3" s="20">
+        <f>140/N7</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="E3" s="20">
+        <f>157/N7</f>
+        <v>1.57E-3</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="N3" s="2">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17">
+        <v>200</v>
+      </c>
+      <c r="C4" s="20">
+        <f>360/N6</f>
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="D4" s="20">
+        <f>297/N7</f>
+        <v>2.97E-3</v>
+      </c>
+      <c r="E4" s="20">
+        <f>421/N7</f>
+        <v>4.2100000000000002E-3</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="24"/>
+      <c r="J4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="N4" s="2">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17">
+        <v>400</v>
+      </c>
+      <c r="C5" s="20">
+        <f>608/N6</f>
+        <v>6.0800000000000003E-4</v>
+      </c>
+      <c r="D5" s="20">
+        <f>625/N7</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="E5" s="20">
+        <f>766/N7</f>
+        <v>7.6600000000000001E-3</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="24"/>
+      <c r="N5" s="2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="17">
+        <v>800</v>
+      </c>
+      <c r="C6" s="20">
+        <f>1164/N6</f>
+        <v>1.1640000000000001E-3</v>
+      </c>
+      <c r="D6" s="20">
+        <f>1228/N7</f>
+        <v>1.2279999999999999E-2</v>
+      </c>
+      <c r="E6" s="20">
+        <f>1497/N7</f>
+        <v>1.4970000000000001E-2</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="24"/>
+      <c r="N6" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17">
+        <v>1600</v>
+      </c>
+      <c r="C7" s="20">
+        <f>2423/N6</f>
+        <v>2.4229999999999998E-3</v>
+      </c>
+      <c r="D7" s="20">
+        <f>2681/N7</f>
+        <v>2.681E-2</v>
+      </c>
+      <c r="E7" s="20">
+        <f>3106/N7</f>
+        <v>3.1060000000000001E-2</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="24"/>
+      <c r="N7" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17">
+        <v>3200</v>
+      </c>
+      <c r="C8" s="20">
+        <f>4863/N6</f>
+        <v>4.8630000000000001E-3</v>
+      </c>
+      <c r="D8" s="20">
+        <f>5666/N7</f>
+        <v>5.6660000000000002E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <f>7963/N7</f>
+        <v>7.9630000000000006E-2</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="24"/>
+      <c r="N8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17">
+        <v>6400</v>
+      </c>
+      <c r="C9" s="20">
+        <f>9550/N6</f>
+        <v>9.5499999999999995E-3</v>
+      </c>
+      <c r="D9" s="20">
+        <f>12639/N7</f>
+        <v>0.12639</v>
+      </c>
+      <c r="E9" s="20">
+        <f>14329/N7</f>
+        <v>0.14329</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="24"/>
+      <c r="N9" s="15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17">
+        <v>12800</v>
+      </c>
+      <c r="C10" s="20">
+        <f>19603/N6</f>
+        <v>1.9602999999999999E-2</v>
+      </c>
+      <c r="D10" s="20">
+        <f>24589/N7</f>
+        <v>0.24589</v>
+      </c>
+      <c r="E10" s="20">
+        <f>28834/N7</f>
+        <v>0.28833999999999999</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="24"/>
+      <c r="N10" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17">
+        <v>25600</v>
+      </c>
+      <c r="C11" s="20">
+        <f>38152/N6</f>
+        <v>3.8151999999999998E-2</v>
+      </c>
+      <c r="D11" s="20">
+        <f>53864/N7</f>
+        <v>0.53864000000000001</v>
+      </c>
+      <c r="E11" s="20">
+        <f>63583/N7</f>
+        <v>0.63583000000000001</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="24"/>
+      <c r="N11" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="17">
+        <v>51200</v>
+      </c>
+      <c r="C12" s="20">
+        <f>76614/N6</f>
+        <v>7.6614000000000002E-2</v>
+      </c>
+      <c r="D12" s="20">
+        <f>109412/N7</f>
+        <v>1.09412</v>
+      </c>
+      <c r="E12" s="20">
+        <f>129514/N7</f>
+        <v>1.29514</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="24"/>
+      <c r="N12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17">
+        <v>102400</v>
+      </c>
+      <c r="C13" s="20">
+        <f>150329/N6</f>
+        <v>0.15032899999999999</v>
+      </c>
+      <c r="D13" s="20">
+        <f>23229/N8</f>
+        <v>2.3229000000000002</v>
+      </c>
+      <c r="E13" s="20">
+        <f>28111/N8</f>
+        <v>2.8111000000000002</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17">
+        <v>204800</v>
+      </c>
+      <c r="C14" s="20">
+        <f>29681/N7</f>
+        <v>0.29681000000000002</v>
+      </c>
+      <c r="D14" s="20">
+        <f>47879/N8</f>
+        <v>4.7878999999999996</v>
+      </c>
+      <c r="E14" s="20">
+        <f>56221/N8</f>
+        <v>5.6220999999999997</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17">
+        <v>409600</v>
+      </c>
+      <c r="C15" s="20">
+        <f>60407/N7</f>
+        <v>0.60407</v>
+      </c>
+      <c r="D15" s="20">
+        <f>102875/N8</f>
+        <v>10.2875</v>
+      </c>
+      <c r="E15" s="20">
+        <f>123641/N8</f>
+        <v>12.364100000000001</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17">
+        <v>819200</v>
+      </c>
+      <c r="C16" s="20">
+        <f>127176/N7</f>
+        <v>1.27176</v>
+      </c>
+      <c r="D16" s="20">
+        <f>23116/N9</f>
+        <v>23.116</v>
+      </c>
+      <c r="E16" s="20">
+        <f>25555/N9</f>
+        <v>25.555</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="17">
+        <v>1638400</v>
+      </c>
+      <c r="C17" s="20">
+        <f>26665/N8</f>
+        <v>2.6665000000000001</v>
+      </c>
+      <c r="D17" s="20">
+        <f>46942/N9</f>
+        <v>46.942</v>
+      </c>
+      <c r="E17" s="20">
+        <f>56089/N9</f>
+        <v>56.088999999999999</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="17">
+        <v>3276800</v>
+      </c>
+      <c r="C18" s="20">
+        <f>53941/N8</f>
+        <v>5.3940999999999999</v>
+      </c>
+      <c r="D18" s="20">
+        <f>94696/N9</f>
+        <v>94.695999999999998</v>
+      </c>
+      <c r="E18" s="20">
+        <f>112740/N9</f>
+        <v>112.74</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="19">
+        <v>6553600</v>
+      </c>
+      <c r="C19" s="20">
+        <f>107396/N8</f>
+        <v>10.739599999999999</v>
+      </c>
+      <c r="D19" s="20">
         <f>21167/N10</f>
         <v>211.67</v>
       </c>
@@ -4247,9 +7884,39 @@
         <v>16</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F051FB6-CA32-4388-85B2-328D80E2ECE0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en las clases (en el excel de la práctica 4 aparece un cambio, pero es porque entre a hacer copia y pega de la columna n para introducirla en la práctica 6, no hay realmente ningún cambio ni toque nada más)
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p4/P4_UO277876.xlsx
+++ b/src/main/java/algestudiante/p4/P4_UO277876.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFBCEC5-7F37-4FC5-BD20-A9A890531239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA3E64F-9A53-4021-89D2-C3A0AC3BE105}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="12144" yWindow="1068" windowWidth="10764" windowHeight="9480" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Devoradores" sheetId="5" r:id="rId1"/>
@@ -6839,7 +6839,7 @@
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G23"/>
+      <selection activeCell="B23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>